<commit_message>
Fix Listado por tiempo
</commit_message>
<xml_diff>
--- a/Excel/Ventas.xlsx
+++ b/Excel/Ventas.xlsx
@@ -97,26 +97,32 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Ventas!$A$2:$A$7</c:f>
+              <c:f>Ventas!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>42400</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>42397</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>42392</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>42395</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>42389</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>42390</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>42401</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>42388</c:v>
                 </c:pt>
               </c:numCache>
@@ -124,26 +130,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ventas!$B$2:$B$7</c:f>
+              <c:f>Ventas!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -544,7 +556,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -564,49 +576,65 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>42397</v>
+        <v>42400</v>
       </c>
       <c r="B2">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>42392</v>
+        <v>42397</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>42395</v>
+        <v>42392</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>42389</v>
+        <v>42395</v>
       </c>
       <c r="B5">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>42390</v>
+        <v>42389</v>
       </c>
       <c r="B6">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
+        <v>42390</v>
+      </c>
+      <c r="B7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2">
+        <v>42401</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2">
         <v>42388</v>
       </c>
-      <c r="B7">
+      <c r="B9">
         <v>3</v>
       </c>
     </row>

</xml_diff>